<commit_message>
Updated notes in the data xls.
</commit_message>
<xml_diff>
--- a/ABMdev/Data/NASS_Data/ID_yield_area_val.xlsx
+++ b/ABMdev/Data/NASS_Data/ID_yield_area_val.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kek25/Documents/GitRepos/IM3-BoiseState/ABMdev/Data/NASS_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kendrakaiser/Documents/GitRepos/IM3-BoiseState/ABMdev/Data/NASS_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6AB3390-578C-A94F-9C85-F37E946417B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14620" yWindow="1000" windowWidth="28180" windowHeight="22000" xr2:uid="{2FF1EF31-B637-584E-9E3D-49C501504A22}"/>
+    <workbookView xWindow="5280" yWindow="6140" windowWidth="41920" windowHeight="19560"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="1990" sheetId="3" r:id="rId3"/>
     <sheet name="2005" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="91">
   <si>
     <t>Data Processing Notes</t>
   </si>
@@ -304,12 +303,15 @@
   </si>
   <si>
     <t>eg at the state level, 2005</t>
+  </si>
+  <si>
+    <t>Scale to the southern region using the 2010 and 2015 data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -662,11 +664,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA7CE003-C972-7147-A0C6-2282FB9BD6A9}">
-  <dimension ref="A1:A36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -706,155 +708,160 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>89</v>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>88</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A11:A35">
-    <sortCondition ref="A11"/>
+  <sortState ref="A12:A36">
+    <sortCondition ref="A12"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7252B790-3F64-1E4B-9C97-C7685DC1802A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1438,11 +1445,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B28FAD4-D7F7-474A-9743-CCEB2D6CB6B6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2151,11 +2158,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9951709-8A31-104A-B4CC-CABE28CAFFB5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+      <selection activeCell="A19" sqref="A19:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2289,7 +2296,7 @@
         <v>49175.87184</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M17" si="4">F4/L4</f>
+        <f t="shared" ref="M4:M11" si="4">F4/L4</f>
         <v>1.3766914030577968</v>
       </c>
     </row>

</xml_diff>